<commit_message>
dfsfdffdsf - Commented GitLatch Commit @ 2025-2-14-16-22-10-79
</commit_message>
<xml_diff>
--- a/test.docx.xlsx
+++ b/test.docx.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F48A47C1-0159-4E48-841B-B3F29CC18F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0352776E-6474-4ABD-BAA9-416AFF1BED4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Hello world</t>
   </si>
   <si>
     <t>sdfsdf</t>
+  </si>
+  <si>
+    <t>hi</t>
   </si>
 </sst>
 </file>
@@ -365,25 +368,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D7:D8"/>
+  <dimension ref="D5:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="7" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>